<commit_message>
Dip & Adm tech names
</commit_message>
<xml_diff>
--- a/planning/techs.xlsx
+++ b/planning/techs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24411"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8156D42C-D62D-42F3-8EA9-BD91B7D4BA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F862293-CC4C-4B39-B29C-80198A9CEB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="206">
   <si>
     <t>notes</t>
   </si>
@@ -283,6 +283,9 @@
     <t>Colonialism</t>
   </si>
   <si>
+    <t>Plantations</t>
+  </si>
+  <si>
     <t>Trading Companies</t>
   </si>
   <si>
@@ -307,6 +310,9 @@
     <t>Steam Pumps</t>
   </si>
   <si>
+    <t>Carracks</t>
+  </si>
+  <si>
     <t>Pike Square</t>
   </si>
   <si>
@@ -331,7 +337,7 @@
     <t>Machinery</t>
   </si>
   <si>
-    <t>Costal Batteries</t>
+    <t>Coastal Batteries</t>
   </si>
   <si>
     <t>Arquebus</t>
@@ -352,7 +358,7 @@
     <t>+0.5 art fire, +0.05 art shock, new art</t>
   </si>
   <si>
-    <t>Textiles</t>
+    <t>Textile Manufactory</t>
   </si>
   <si>
     <t>Steamers</t>
@@ -367,6 +373,9 @@
     <t>Colonial Thought</t>
   </si>
   <si>
+    <t>Colonial Charters</t>
+  </si>
+  <si>
     <t>Weapons Manufactory</t>
   </si>
   <si>
@@ -388,6 +397,9 @@
     <t>+0.2 inf fire, 3 combat width</t>
   </si>
   <si>
+    <t>Modern Metallurgy</t>
+  </si>
+  <si>
     <t>Lineships</t>
   </si>
   <si>
@@ -397,7 +409,10 @@
     <t>+0.25 tactics, +0.2 inf fire</t>
   </si>
   <si>
-    <t>Scientific Enquirer</t>
+    <t>Scientific Enquiry</t>
+  </si>
+  <si>
+    <t>Screw Propeller</t>
   </si>
   <si>
     <t>Trunnions</t>
@@ -409,6 +424,9 @@
     <t>Military Administration</t>
   </si>
   <si>
+    <t>Merchantman</t>
+  </si>
+  <si>
     <t>Volley fire</t>
   </si>
   <si>
@@ -442,6 +460,12 @@
     <t>Bastions Building (Level 4 fort)</t>
   </si>
   <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Threedeckers</t>
+  </si>
+  <si>
     <t>Standardization</t>
   </si>
   <si>
@@ -454,6 +478,9 @@
     <t>Religious Edifice</t>
   </si>
   <si>
+    <t>Naval Proffessionalization</t>
+  </si>
+  <si>
     <t>Air Ships</t>
   </si>
   <si>
@@ -463,6 +490,9 @@
     <t>Rights of Nations</t>
   </si>
   <si>
+    <t>Steam Turbine</t>
+  </si>
+  <si>
     <t>Killing Grounds</t>
   </si>
   <si>
@@ -472,6 +502,9 @@
     <t>New Thought</t>
   </si>
   <si>
+    <t>Merchant Vessels</t>
+  </si>
+  <si>
     <t>Steam air ships</t>
   </si>
   <si>
@@ -481,6 +514,9 @@
     <t>Land Clearance</t>
   </si>
   <si>
+    <t>All-or-Nothing Armor Scheme</t>
+  </si>
+  <si>
     <t>Ankon Armor</t>
   </si>
   <si>
@@ -493,6 +529,9 @@
     <t>Rights of Mortals</t>
   </si>
   <si>
+    <t>Joint Stock Companies</t>
+  </si>
+  <si>
     <t>Specialized Regiments</t>
   </si>
   <si>
@@ -502,7 +541,10 @@
     <t>Industrial Production</t>
   </si>
   <si>
-    <t>Breach-loading</t>
+    <t>Public Punishments</t>
+  </si>
+  <si>
+    <t>Breech-loading</t>
   </si>
   <si>
     <t>+1.0 art fire, +1.0 cav fire, new arty</t>
@@ -538,7 +580,7 @@
     <t>Mesurements and Weights</t>
   </si>
   <si>
-    <t>Joint Stock Companies</t>
+    <t>Cargo Ships</t>
   </si>
   <si>
     <t>Covered Way</t>
@@ -559,7 +601,7 @@
     <t>+2.0 cav fire, +4.0 cav shock, new cav</t>
   </si>
   <si>
-    <t>Four Field Rotation</t>
+    <t>Railroads</t>
   </si>
   <si>
     <t>Battleships</t>
@@ -577,19 +619,25 @@
     <t>Silver Standard</t>
   </si>
   <si>
-    <t>Rifle</t>
-  </si>
-  <si>
-    <t>+0.5 inf fire, +50% supply limit, +25% flanking range</t>
-  </si>
-  <si>
-    <t>High Caliber guns</t>
-  </si>
-  <si>
-    <t>Field Howitzers</t>
+    <t>Lile Rifle</t>
+  </si>
+  <si>
+    <t>+0.5 inf fire, +50% supply limit, +25% flanking range, new inf</t>
+  </si>
+  <si>
+    <t>Mechanized Mining</t>
+  </si>
+  <si>
+    <t>Market Regulation</t>
+  </si>
+  <si>
+    <t>Rifled Artillery</t>
   </si>
   <si>
     <t>+2.0 art fire, +1.0 cav fire</t>
+  </si>
+  <si>
+    <t>Tractors</t>
   </si>
   <si>
     <t>Superfiring Armaments</t>
@@ -932,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1311,14 +1359,17 @@
         <f t="shared" si="0"/>
         <v>1456</v>
       </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1327,16 +1378,16 @@
         <v>1469</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1345,13 +1396,16 @@
         <v>1482</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
       </c>
       <c r="G21" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1360,40 +1414,40 @@
         <v>1495</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
         <v>1508</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1402,16 +1456,16 @@
         <v>1521</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1420,16 +1474,16 @@
         <v>1534</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1438,37 +1492,40 @@
         <v>1547</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
       </c>
+      <c r="E26" t="s">
+        <v>114</v>
+      </c>
       <c r="G26" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H26" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
         <v>1560</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G27" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1476,14 +1533,17 @@
         <f t="shared" si="0"/>
         <v>1573</v>
       </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
       <c r="E28" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G28" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H28" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1492,13 +1552,16 @@
         <v>1586</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>126</v>
+      </c>
+      <c r="E29" t="s">
+        <v>127</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="H29" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1507,37 +1570,40 @@
         <v>1599</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>130</v>
+      </c>
+      <c r="E30" t="s">
+        <v>131</v>
       </c>
       <c r="G30" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H30" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
         <v>1612</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
         <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G31" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H31" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1546,16 +1612,16 @@
         <v>1625</v>
       </c>
       <c r="C32" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G32" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H32" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1563,29 +1629,38 @@
         <f t="shared" si="0"/>
         <v>1638</v>
       </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" t="s">
+        <v>144</v>
+      </c>
       <c r="G33" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="H33" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
         <v>1651</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>148</v>
+      </c>
+      <c r="E34" t="s">
+        <v>149</v>
       </c>
       <c r="G34" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="H34" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1594,16 +1669,19 @@
         <v>1664</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D35" t="s">
         <v>25</v>
       </c>
+      <c r="E35" t="s">
+        <v>153</v>
+      </c>
       <c r="G35" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="H35" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1612,13 +1690,16 @@
         <v>1677</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>156</v>
+      </c>
+      <c r="E36" t="s">
+        <v>157</v>
       </c>
       <c r="G36" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="H36" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1627,34 +1708,40 @@
         <v>1690</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>160</v>
+      </c>
+      <c r="E37" t="s">
+        <v>161</v>
       </c>
       <c r="G37" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="H37" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
         <v>1703</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="D38" t="s">
         <v>25</v>
       </c>
+      <c r="E38" t="s">
+        <v>166</v>
+      </c>
       <c r="G38" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="H38" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1663,13 +1750,16 @@
         <v>1716</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>169</v>
+      </c>
+      <c r="E39" t="s">
+        <v>170</v>
       </c>
       <c r="G39" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="H39" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1678,16 +1768,16 @@
         <v>1729</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="E40" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="G40" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="H40" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1696,40 +1786,40 @@
         <v>1742</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="G41" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="H41" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
         <v>1755</v>
       </c>
       <c r="C42" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E42" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="G42" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="H42" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1738,16 +1828,16 @@
         <v>1768</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="G43" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="H43" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1756,16 +1846,16 @@
         <v>1781</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="E44" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="G44" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="H44" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1774,19 +1864,19 @@
         <v>1794</v>
       </c>
       <c r="C45" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D45" t="s">
         <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G45" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="H45" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1794,14 +1884,17 @@
         <f t="shared" si="0"/>
         <v>1807</v>
       </c>
+      <c r="C46" t="s">
+        <v>198</v>
+      </c>
       <c r="E46" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="G46" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="H46" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1809,14 +1902,17 @@
         <f t="shared" si="0"/>
         <v>1820</v>
       </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
       <c r="E47" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="G47" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="H47" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start of the kolbold units
</commit_message>
<xml_diff>
--- a/planning/techs.xlsx
+++ b/planning/techs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -838,11 +838,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -2322,75 +2322,6 @@
                 <c:pt idx="19">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>14</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5288,11 +5219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106838272"/>
-        <c:axId val="106079744"/>
+        <c:axId val="82166144"/>
+        <c:axId val="82164352"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="106079744"/>
+        <c:axId val="82164352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -5306,12 +5237,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106838272"/>
+        <c:crossAx val="82166144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="106838272"/>
+        <c:axId val="82166144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5345,7 +5276,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106079744"/>
+        <c:crossAx val="82164352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7426,11 +7357,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72906240"/>
-        <c:axId val="72907776"/>
+        <c:axId val="88204800"/>
+        <c:axId val="88206336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72906240"/>
+        <c:axId val="88204800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7440,7 +7371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72907776"/>
+        <c:crossAx val="88206336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7448,7 +7379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72907776"/>
+        <c:axId val="88206336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -7460,7 +7391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72906240"/>
+        <c:crossAx val="88204800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7802,7 +7733,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8757,8 +8688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8778,35 +8709,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -8859,7 +8790,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="3">
@@ -8868,10 +8799,10 @@
       <c r="C3" s="3">
         <v>5</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>5</v>
       </c>
       <c r="F3" s="3">
@@ -8886,25 +8817,25 @@
       <c r="J3" s="3">
         <v>3</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="6"/>
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="3">
         <v>4</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="3">
         <v>4</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="6">
         <v>6</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4">
@@ -8948,7 +8879,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5">
@@ -9036,7 +8967,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7">
@@ -9045,10 +8976,10 @@
       <c r="C7" s="3">
         <v>6</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>6</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>6</v>
       </c>
       <c r="F7">
@@ -9069,7 +9000,7 @@
       <c r="M7">
         <v>4</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="3">
         <v>5</v>
       </c>
       <c r="O7">
@@ -9080,7 +9011,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8">
@@ -9110,7 +9041,7 @@
       <c r="L8">
         <v>4</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="3">
         <v>6</v>
       </c>
       <c r="N8">
@@ -9119,7 +9050,7 @@
       <c r="O8">
         <v>6</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="6">
         <v>7</v>
       </c>
     </row>
@@ -9168,7 +9099,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10">
@@ -9186,7 +9117,7 @@
       <c r="F10" s="3">
         <v>7</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>7</v>
       </c>
       <c r="H10">
@@ -9207,7 +9138,7 @@
       <c r="N10">
         <v>5</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="6">
         <v>8</v>
       </c>
       <c r="P10">
@@ -9215,7 +9146,7 @@
       </c>
     </row>
     <row r="11" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11">
@@ -9248,10 +9179,10 @@
       <c r="L11" s="3">
         <v>5</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="3">
         <v>7</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="3">
         <v>7</v>
       </c>
       <c r="O11">
@@ -9262,7 +9193,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12">
@@ -9271,10 +9202,10 @@
       <c r="C12" s="3">
         <v>7</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>7</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>7</v>
       </c>
       <c r="F12">
@@ -9304,7 +9235,7 @@
       <c r="O12">
         <v>8</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <v>8</v>
       </c>
     </row>
@@ -9403,7 +9334,7 @@
       </c>
     </row>
     <row r="15" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15">
@@ -9436,7 +9367,7 @@
       <c r="L15" s="3">
         <v>8</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="3">
         <v>8</v>
       </c>
       <c r="N15">
@@ -9445,12 +9376,12 @@
       <c r="O15">
         <v>8</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16">
@@ -9486,10 +9417,10 @@
       <c r="M16">
         <v>8</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <v>8</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <v>10</v>
       </c>
       <c r="P16">
@@ -9497,7 +9428,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17">
@@ -9506,10 +9437,10 @@
       <c r="C17" s="3">
         <v>8</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>8</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>8</v>
       </c>
       <c r="F17">
@@ -9539,7 +9470,7 @@
       <c r="O17">
         <v>10</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="6">
         <v>10</v>
       </c>
     </row>
@@ -9577,7 +9508,7 @@
       <c r="L18">
         <v>8</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="6">
         <v>11</v>
       </c>
       <c r="N18">
@@ -9591,7 +9522,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19">
@@ -9606,7 +9537,7 @@
       <c r="E19">
         <v>8</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>12</v>
       </c>
       <c r="G19" s="3">
@@ -9627,7 +9558,7 @@
       <c r="M19">
         <v>11</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="6">
         <v>11</v>
       </c>
       <c r="O19">
@@ -9638,7 +9569,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20">
@@ -9647,10 +9578,10 @@
       <c r="C20" s="3">
         <v>12</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>12</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>12</v>
       </c>
       <c r="F20">
@@ -9685,7 +9616,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21">
@@ -9724,15 +9655,15 @@
       <c r="N21">
         <v>11</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="6">
         <v>12</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22">
@@ -9747,7 +9678,7 @@
       <c r="E22">
         <v>12</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>14</v>
       </c>
       <c r="G22" s="3">
@@ -9765,10 +9696,10 @@
       <c r="L22">
         <v>10</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="6">
         <v>13</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="6">
         <v>13</v>
       </c>
       <c r="O22">
@@ -9779,7 +9710,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23">
@@ -9788,14 +9719,11 @@
       <c r="C23" s="3">
         <v>16</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>16</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>16</v>
-      </c>
-      <c r="F23">
-        <v>14</v>
       </c>
       <c r="G23">
         <v>16</v>
@@ -9841,9 +9769,6 @@
       <c r="E24">
         <v>16</v>
       </c>
-      <c r="F24">
-        <v>14</v>
-      </c>
       <c r="G24">
         <v>16</v>
       </c>
@@ -9873,7 +9798,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25">
@@ -9888,9 +9813,6 @@
       <c r="E25">
         <v>16</v>
       </c>
-      <c r="F25">
-        <v>14</v>
-      </c>
       <c r="G25" s="3">
         <v>17</v>
       </c>
@@ -9915,7 +9837,7 @@
       <c r="O25">
         <v>12</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="6">
         <v>16</v>
       </c>
     </row>
@@ -9935,9 +9857,6 @@
       <c r="E26">
         <v>16</v>
       </c>
-      <c r="F26">
-        <v>14</v>
-      </c>
       <c r="G26">
         <v>17</v>
       </c>
@@ -9959,7 +9878,7 @@
       <c r="N26">
         <v>13</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="6">
         <v>14</v>
       </c>
       <c r="P26">
@@ -9967,7 +9886,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27">
@@ -9976,14 +9895,11 @@
       <c r="C27" s="3">
         <v>19</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>18</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>19</v>
-      </c>
-      <c r="F27">
-        <v>14</v>
       </c>
       <c r="G27">
         <v>17</v>
@@ -10000,16 +9916,16 @@
       <c r="L27" s="3">
         <v>14</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="6">
         <v>17</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="6">
         <v>18</v>
       </c>
       <c r="O27">
         <v>14</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="6">
         <v>19</v>
       </c>
     </row>
@@ -10029,9 +9945,6 @@
       <c r="E28">
         <v>19</v>
       </c>
-      <c r="F28">
-        <v>14</v>
-      </c>
       <c r="G28">
         <v>17</v>
       </c>
@@ -10076,9 +9989,6 @@
       <c r="E29">
         <v>19</v>
       </c>
-      <c r="F29">
-        <v>14</v>
-      </c>
       <c r="G29">
         <v>17</v>
       </c>
@@ -10108,7 +10018,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30">
@@ -10123,9 +10033,6 @@
       <c r="E30">
         <v>19</v>
       </c>
-      <c r="F30">
-        <v>14</v>
-      </c>
       <c r="G30">
         <v>17</v>
       </c>
@@ -10150,12 +10057,12 @@
       <c r="O30">
         <v>14</v>
       </c>
-      <c r="P30" s="7">
+      <c r="P30" s="6">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31">
@@ -10164,14 +10071,11 @@
       <c r="C31" s="3">
         <v>22</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>21</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>22</v>
-      </c>
-      <c r="F31">
-        <v>14</v>
       </c>
       <c r="G31" s="3">
         <v>22</v>
@@ -10188,10 +10092,10 @@
       <c r="L31" s="3">
         <v>18</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="6">
         <v>20</v>
       </c>
-      <c r="N31" s="7">
+      <c r="N31" s="6">
         <v>21</v>
       </c>
       <c r="O31">
@@ -10202,7 +10106,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32">
@@ -10217,9 +10121,6 @@
       <c r="E32">
         <v>22</v>
       </c>
-      <c r="F32">
-        <v>14</v>
-      </c>
       <c r="G32">
         <v>22</v>
       </c>
@@ -10241,7 +10142,7 @@
       <c r="N32">
         <v>21</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="6">
         <v>18</v>
       </c>
       <c r="P32">
@@ -10264,9 +10165,6 @@
       <c r="E33">
         <v>22</v>
       </c>
-      <c r="F33">
-        <v>14</v>
-      </c>
       <c r="G33">
         <v>22</v>
       </c>
@@ -10296,7 +10194,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34">
@@ -10310,9 +10208,6 @@
       </c>
       <c r="E34">
         <v>22</v>
-      </c>
-      <c r="F34">
-        <v>14</v>
       </c>
       <c r="G34">
         <v>22</v>
@@ -10358,9 +10253,6 @@
       <c r="E35">
         <v>22</v>
       </c>
-      <c r="F35">
-        <v>14</v>
-      </c>
       <c r="G35">
         <v>22</v>
       </c>
@@ -10405,9 +10297,6 @@
       <c r="E36">
         <v>22</v>
       </c>
-      <c r="F36">
-        <v>14</v>
-      </c>
       <c r="G36">
         <v>22</v>
       </c>
@@ -10437,7 +10326,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37">
@@ -10446,14 +10335,11 @@
       <c r="C37" s="3">
         <v>26</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>27</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>26</v>
-      </c>
-      <c r="F37">
-        <v>14</v>
       </c>
       <c r="G37" s="3">
         <v>26</v>
@@ -10470,7 +10356,7 @@
       <c r="L37">
         <v>22</v>
       </c>
-      <c r="M37" s="7">
+      <c r="M37" s="6">
         <v>25</v>
       </c>
       <c r="N37">
@@ -10479,12 +10365,12 @@
       <c r="O37">
         <v>18</v>
       </c>
-      <c r="P37" s="7">
+      <c r="P37" s="6">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38">
@@ -10499,9 +10385,6 @@
       <c r="E38">
         <v>26</v>
       </c>
-      <c r="F38">
-        <v>14</v>
-      </c>
       <c r="G38">
         <v>26</v>
       </c>
@@ -10520,10 +10403,10 @@
       <c r="M38">
         <v>25</v>
       </c>
-      <c r="N38" s="7">
+      <c r="N38" s="6">
         <v>26</v>
       </c>
-      <c r="O38" s="7">
+      <c r="O38" s="6">
         <v>22</v>
       </c>
       <c r="P38">
@@ -10531,7 +10414,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39">
@@ -10546,9 +10429,6 @@
       <c r="E39">
         <v>26</v>
       </c>
-      <c r="F39">
-        <v>14</v>
-      </c>
       <c r="G39">
         <v>26</v>
       </c>
@@ -10573,7 +10453,7 @@
       <c r="O39">
         <v>22</v>
       </c>
-      <c r="P39" s="7">
+      <c r="P39" s="6">
         <v>28</v>
       </c>
     </row>
@@ -10593,9 +10473,6 @@
       <c r="E40">
         <v>26</v>
       </c>
-      <c r="F40">
-        <v>14</v>
-      </c>
       <c r="G40">
         <v>26</v>
       </c>
@@ -10625,7 +10502,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41">
@@ -10634,14 +10511,11 @@
       <c r="C41" s="3">
         <v>30</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="6">
         <v>31</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="6">
         <v>30</v>
-      </c>
-      <c r="F41">
-        <v>14</v>
       </c>
       <c r="G41" s="3">
         <v>30</v>
@@ -10658,16 +10532,16 @@
       <c r="L41" s="3">
         <v>29</v>
       </c>
-      <c r="M41" s="7">
+      <c r="M41" s="6">
         <v>29</v>
       </c>
-      <c r="N41" s="7">
+      <c r="N41" s="6">
         <v>30</v>
       </c>
-      <c r="O41" s="7">
+      <c r="O41" s="6">
         <v>29</v>
       </c>
-      <c r="P41" s="7">
+      <c r="P41" s="3">
         <v>30</v>
       </c>
     </row>
@@ -10687,9 +10561,6 @@
       <c r="E42">
         <v>30</v>
       </c>
-      <c r="F42">
-        <v>14</v>
-      </c>
       <c r="G42">
         <v>30</v>
       </c>
@@ -10734,9 +10605,6 @@
       <c r="E43">
         <v>30</v>
       </c>
-      <c r="F43">
-        <v>14</v>
-      </c>
       <c r="G43">
         <v>30</v>
       </c>
@@ -10781,9 +10649,6 @@
       <c r="E44">
         <v>30</v>
       </c>
-      <c r="F44">
-        <v>14</v>
-      </c>
       <c r="G44">
         <v>30</v>
       </c>
@@ -10813,7 +10678,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45">
@@ -10822,14 +10687,11 @@
       <c r="C45" s="3">
         <v>34</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>35</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>34</v>
-      </c>
-      <c r="F45">
-        <v>14</v>
       </c>
       <c r="G45" s="3">
         <v>34</v>
@@ -10846,16 +10708,16 @@
       <c r="L45" s="3">
         <v>32</v>
       </c>
-      <c r="M45" s="7">
+      <c r="M45" s="6">
         <v>33</v>
       </c>
-      <c r="N45" s="7">
+      <c r="N45" s="6">
         <v>34</v>
       </c>
-      <c r="O45" s="7">
+      <c r="O45" s="6">
         <v>33</v>
       </c>
-      <c r="P45" s="7">
+      <c r="P45" s="6">
         <v>33</v>
       </c>
     </row>
@@ -10863,41 +10725,41 @@
       <c r="A46">
         <v>46</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="6">
         <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
-      <c r="P89" s="5"/>
-      <c r="Q89" s="5"/>
-      <c r="R89" s="5"/>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="5"/>
-      <c r="V89" s="5"/>
-      <c r="W89" s="5"/>
-      <c r="X89" s="5"/>
-      <c r="Y89" s="5"/>
-      <c r="Z89" s="5"/>
-      <c r="AA89" s="5"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="7"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="7"/>
+      <c r="P89" s="7"/>
+      <c r="Q89" s="7"/>
+      <c r="R89" s="7"/>
+      <c r="S89" s="7"/>
+      <c r="T89" s="7"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+      <c r="W89" s="7"/>
+      <c r="X89" s="7"/>
+      <c r="Y89" s="7"/>
+      <c r="Z89" s="7"/>
+      <c r="AA89" s="7"/>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">

</xml_diff>

<commit_message>
finishing kolbold units and other additions
finished rake/kolbolds, free kolbolds and dunirr infantry units
added bronze-age leagues
Oayvein is now a grand duchy
</commit_message>
<xml_diff>
--- a/planning/techs.xlsx
+++ b/planning/techs.xlsx
@@ -3692,6 +3692,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5202,7 +5205,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5219,11 +5222,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82166144"/>
-        <c:axId val="82164352"/>
+        <c:axId val="41369600"/>
+        <c:axId val="41367808"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="82164352"/>
+        <c:axId val="41367808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -5237,12 +5240,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82166144"/>
+        <c:crossAx val="41369600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="82166144"/>
+        <c:axId val="41369600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5276,7 +5279,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82164352"/>
+        <c:crossAx val="41367808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7357,11 +7360,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88204800"/>
-        <c:axId val="88206336"/>
+        <c:axId val="41510016"/>
+        <c:axId val="41511552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88204800"/>
+        <c:axId val="41510016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7371,7 +7374,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88206336"/>
+        <c:crossAx val="41511552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7379,7 +7382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88206336"/>
+        <c:axId val="41511552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -7391,7 +7394,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88204800"/>
+        <c:crossAx val="41510016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7733,7 +7736,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8688,8 +8691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8817,7 +8820,9 @@
       <c r="J3" s="3">
         <v>3</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6">
+        <v>3</v>
+      </c>
       <c r="L3">
         <v>1</v>
       </c>
@@ -8830,7 +8835,7 @@
       <c r="O3" s="6">
         <v>6</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="3">
         <v>5</v>
       </c>
     </row>
@@ -8841,7 +8846,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>5</v>
       </c>
       <c r="D4">
@@ -9010,7 +9015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -9050,11 +9055,11 @@
       <c r="O8">
         <v>6</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9235,7 +9240,7 @@
       <c r="O12">
         <v>8</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="3">
         <v>8</v>
       </c>
     </row>
@@ -9286,7 +9291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9333,7 +9338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -9376,7 +9381,7 @@
       <c r="O15">
         <v>8</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="3">
         <v>9</v>
       </c>
     </row>
@@ -9417,7 +9422,7 @@
       <c r="M16">
         <v>8</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="3">
         <v>8</v>
       </c>
       <c r="O16" s="6">
@@ -9470,7 +9475,7 @@
       <c r="O17">
         <v>10</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="3">
         <v>10</v>
       </c>
     </row>
@@ -9508,7 +9513,7 @@
       <c r="L18">
         <v>8</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="3">
         <v>11</v>
       </c>
       <c r="N18">
@@ -9558,7 +9563,7 @@
       <c r="M19">
         <v>11</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="3">
         <v>11</v>
       </c>
       <c r="O19">
@@ -9658,7 +9663,7 @@
       <c r="O21" s="6">
         <v>12</v>
       </c>
-      <c r="P21" s="6">
+      <c r="P21" s="3">
         <v>14</v>
       </c>
     </row>
@@ -9696,10 +9701,10 @@
       <c r="L22">
         <v>10</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="3">
         <v>13</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="3">
         <v>13</v>
       </c>
       <c r="O22">
@@ -9753,7 +9758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9797,7 +9802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9837,7 +9842,7 @@
       <c r="O25">
         <v>12</v>
       </c>
-      <c r="P25" s="6">
+      <c r="P25" s="3">
         <v>16</v>
       </c>
     </row>
@@ -9916,16 +9921,16 @@
       <c r="L27" s="3">
         <v>14</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M27" s="3">
         <v>17</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="3">
         <v>18</v>
       </c>
       <c r="O27">
         <v>14</v>
       </c>
-      <c r="P27" s="6">
+      <c r="P27" s="3">
         <v>19</v>
       </c>
     </row>
@@ -9973,7 +9978,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10017,7 +10022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -10057,7 +10062,7 @@
       <c r="O30">
         <v>14</v>
       </c>
-      <c r="P30" s="6">
+      <c r="P30" s="3">
         <v>22</v>
       </c>
     </row>
@@ -10092,10 +10097,10 @@
       <c r="L31" s="3">
         <v>18</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31" s="3">
         <v>20</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="3">
         <v>21</v>
       </c>
       <c r="O31">
@@ -10356,7 +10361,7 @@
       <c r="L37">
         <v>22</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="3">
         <v>25</v>
       </c>
       <c r="N37">
@@ -10365,7 +10370,7 @@
       <c r="O37">
         <v>18</v>
       </c>
-      <c r="P37" s="6">
+      <c r="P37" s="3">
         <v>26</v>
       </c>
     </row>
@@ -10403,7 +10408,7 @@
       <c r="M38">
         <v>25</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="3">
         <v>26</v>
       </c>
       <c r="O38" s="6">
@@ -10413,7 +10418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -10453,11 +10458,11 @@
       <c r="O39">
         <v>22</v>
       </c>
-      <c r="P39" s="6">
+      <c r="P39" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10532,10 +10537,10 @@
       <c r="L41" s="3">
         <v>29</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41" s="3">
         <v>29</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N41" s="3">
         <v>30</v>
       </c>
       <c r="O41" s="6">
@@ -10708,17 +10713,17 @@
       <c r="L45" s="3">
         <v>32</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45" s="3">
         <v>33</v>
       </c>
-      <c r="N45" s="6">
+      <c r="N45" s="3">
         <v>34</v>
       </c>
       <c r="O45" s="6">
         <v>33</v>
       </c>
-      <c r="P45" s="6">
-        <v>33</v>
+      <c r="P45" s="3">
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
massive amounts of changes
lore stuff
added the nagas in
buff the hirdam order
fixed the federate war goal
fixed the sea elf leader namelists
reworked the colonial regions in elteria again
added the deepgrove region in n. elteria
finished the planning for the expeditions and started adding them
added trees around the map
added steppes to certain regions
fixed the river in the redmarsh->timberia
the strongholders event chain can now start
</commit_message>
<xml_diff>
--- a/planning/techs.xlsx
+++ b/planning/techs.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="233">
   <si>
     <t>notes</t>
   </si>
@@ -759,6 +759,33 @@
   </si>
   <si>
     <t>Generic</t>
+  </si>
+  <si>
+    <t>Spiders, Ugluk, Settled Humans</t>
+  </si>
+  <si>
+    <t>Spiders, Ugluk, Settled Humans, Elves</t>
+  </si>
+  <si>
+    <t>Settled Humans</t>
+  </si>
+  <si>
+    <t>Settled Humans, Spiders</t>
+  </si>
+  <si>
+    <t>Dunirr, Moon Elves, Lake Elves, Ulguir</t>
+  </si>
+  <si>
+    <t>Dunirr, Ulguir, Settled Humans, Moon Elves, Lake Elves</t>
+  </si>
+  <si>
+    <t>Dunirr, Ulguir, Settled Humans, Moon Elves, Lake Elves, Scurians</t>
+  </si>
+  <si>
+    <t>Sun Elves</t>
+  </si>
+  <si>
+    <t>Spiders, Ugluk</t>
   </si>
 </sst>
 </file>
@@ -5419,11 +5446,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45728128"/>
-        <c:axId val="45722240"/>
+        <c:axId val="65781760"/>
+        <c:axId val="65775872"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="45722240"/>
+        <c:axId val="65775872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -5437,12 +5464,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45728128"/>
+        <c:crossAx val="65781760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="45728128"/>
+        <c:axId val="65781760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5469,14 +5496,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45722240"/>
+        <c:crossAx val="65775872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5486,7 +5512,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7557,11 +7582,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="46126592"/>
-        <c:axId val="46128128"/>
+        <c:axId val="66704512"/>
+        <c:axId val="66706048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46126592"/>
+        <c:axId val="66704512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7571,7 +7596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46128128"/>
+        <c:crossAx val="66706048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7579,7 +7604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46128128"/>
+        <c:axId val="66706048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -7591,7 +7616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46126592"/>
+        <c:crossAx val="66704512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8887,8 +8912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="W45" sqref="W45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9034,6 +9059,9 @@
       <c r="P3" s="3">
         <v>5</v>
       </c>
+      <c r="U3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -9081,6 +9109,9 @@
       <c r="P4">
         <v>5</v>
       </c>
+      <c r="U4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -9128,6 +9159,9 @@
       <c r="P5">
         <v>5</v>
       </c>
+      <c r="U5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -9175,6 +9209,9 @@
       <c r="P6">
         <v>5</v>
       </c>
+      <c r="U6" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
@@ -9222,6 +9259,9 @@
       <c r="P7">
         <v>5</v>
       </c>
+      <c r="U7" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="8" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
@@ -9269,6 +9309,9 @@
       <c r="P8" s="3">
         <v>7</v>
       </c>
+      <c r="U8" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -9316,6 +9359,9 @@
       <c r="P9">
         <v>7</v>
       </c>
+      <c r="U9" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
@@ -9366,6 +9412,9 @@
       <c r="P10">
         <v>7</v>
       </c>
+      <c r="U10" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="11" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
@@ -9416,6 +9465,9 @@
       <c r="P11">
         <v>7</v>
       </c>
+      <c r="U11" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -9466,6 +9518,9 @@
       <c r="P12" s="3">
         <v>8</v>
       </c>
+      <c r="U12" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -9516,6 +9571,9 @@
       <c r="P13">
         <v>8</v>
       </c>
+      <c r="U13" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -9566,6 +9624,9 @@
       <c r="P14">
         <v>8</v>
       </c>
+      <c r="U14" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="15" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
@@ -9616,6 +9677,9 @@
       <c r="P15" s="3">
         <v>9</v>
       </c>
+      <c r="U15" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -9666,8 +9730,11 @@
       <c r="P16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -9716,8 +9783,11 @@
       <c r="P17" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -9766,8 +9836,11 @@
       <c r="P18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -9816,8 +9889,11 @@
       <c r="P19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -9866,8 +9942,11 @@
       <c r="P20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9916,8 +9995,11 @@
       <c r="P21" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -9966,8 +10048,11 @@
       <c r="P22">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -10013,8 +10098,11 @@
       <c r="P23">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10060,8 +10148,11 @@
       <c r="P24">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -10107,8 +10198,11 @@
       <c r="P25" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10154,8 +10248,11 @@
       <c r="P26">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -10201,8 +10298,11 @@
       <c r="P27" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10248,8 +10348,11 @@
       <c r="P28">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10295,8 +10398,11 @@
       <c r="P29">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U29" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -10342,8 +10448,11 @@
       <c r="P30" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -10389,8 +10498,11 @@
       <c r="P31">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U31" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -10436,8 +10548,11 @@
       <c r="P32">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10483,8 +10598,11 @@
       <c r="P33">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U33" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -10530,8 +10648,11 @@
       <c r="P34">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U34" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10577,8 +10698,11 @@
       <c r="P35">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10624,8 +10748,11 @@
       <c r="P36">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -10671,8 +10798,11 @@
       <c r="P37" s="3">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -10718,8 +10848,11 @@
       <c r="P38">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -10765,8 +10898,11 @@
       <c r="P39" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U39" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10812,8 +10948,11 @@
       <c r="P40">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -10859,8 +10998,11 @@
       <c r="P41" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U41" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10906,8 +11048,11 @@
       <c r="P42">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10953,8 +11098,11 @@
       <c r="P43">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11000,8 +11148,11 @@
       <c r="P44">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U44" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -11047,8 +11198,11 @@
       <c r="P45" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U45" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -11057,6 +11211,9 @@
       </c>
       <c r="H46" s="3">
         <v>35</v>
+      </c>
+      <c r="U46" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
eras and other tweaks
</commit_message>
<xml_diff>
--- a/planning/techs.xlsx
+++ b/planning/techs.xlsx
@@ -5446,11 +5446,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="65781760"/>
-        <c:axId val="65775872"/>
+        <c:axId val="59293696"/>
+        <c:axId val="59287808"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="65775872"/>
+        <c:axId val="59287808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35"/>
@@ -5464,12 +5464,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65781760"/>
+        <c:crossAx val="59293696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="65781760"/>
+        <c:axId val="59293696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5496,13 +5496,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65775872"/>
+        <c:crossAx val="59287808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5512,6 +5513,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7582,11 +7584,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66704512"/>
-        <c:axId val="66706048"/>
+        <c:axId val="59692160"/>
+        <c:axId val="59693696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66704512"/>
+        <c:axId val="59692160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7596,7 +7598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66706048"/>
+        <c:crossAx val="59693696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7604,7 +7606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66706048"/>
+        <c:axId val="59693696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -7616,7 +7618,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66704512"/>
+        <c:crossAx val="59692160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7957,7 +7959,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8912,8 +8914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9946,7 +9948,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9989,7 +9991,7 @@
       <c r="N21">
         <v>11</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="3">
         <v>12</v>
       </c>
       <c r="P21" s="3">
@@ -9999,7 +10001,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -10152,7 +10154,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -10202,7 +10204,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10242,7 +10244,7 @@
       <c r="N26">
         <v>13</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="3">
         <v>14</v>
       </c>
       <c r="P26">
@@ -10502,7 +10504,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -10542,7 +10544,7 @@
       <c r="N32">
         <v>21</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="3">
         <v>18</v>
       </c>
       <c r="P32">
@@ -10552,7 +10554,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10802,7 +10804,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -10842,7 +10844,7 @@
       <c r="N38" s="3">
         <v>26</v>
       </c>
-      <c r="O38" s="6">
+      <c r="O38" s="3">
         <v>22</v>
       </c>
       <c r="P38">
@@ -10852,7 +10854,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -10992,7 +10994,7 @@
       <c r="N41" s="3">
         <v>30</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="3">
         <v>29</v>
       </c>
       <c r="P41" s="3">
@@ -11192,7 +11194,7 @@
       <c r="N45" s="3">
         <v>34</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="3">
         <v>33</v>
       </c>
       <c r="P45" s="3">

</xml_diff>